<commit_message>
User 1 added to cell A3
</commit_message>
<xml_diff>
--- a/MyExcelFile.xlsx
+++ b/MyExcelFile.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>This is the original Excel file!</t>
+  </si>
+  <si>
+    <t>User 1 added something in cell A3</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,6 +371,11 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User 2 addde something to cell A4
</commit_message>
<xml_diff>
--- a/MyExcelFile.xlsx
+++ b/MyExcelFile.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>This is the original Excel file!</t>
+  </si>
+  <si>
+    <t>User 2 added something in cell A4</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,6 +371,11 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert change from user 2
</commit_message>
<xml_diff>
--- a/MyExcelFile.xlsx
+++ b/MyExcelFile.xlsx
@@ -21,7 +21,7 @@
     <t>This is the original Excel file!</t>
   </si>
   <si>
-    <t>User 2 added something in cell A4</t>
+    <t>User 1 added something in cell A3</t>
   </si>
 </sst>
 </file>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,8 +373,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
User 2 adds something
</commit_message>
<xml_diff>
--- a/MyExcelFile.xlsx
+++ b/MyExcelFile.xlsx
@@ -21,7 +21,7 @@
     <t>This is the original Excel file!</t>
   </si>
   <si>
-    <t>User 2 added something in cell A4</t>
+    <t>User 2 added something in cell A4!</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>